<commit_message>
updated self evaluation file
</commit_message>
<xml_diff>
--- a/2024_2025_proj_auto_avaliacao.xlsx
+++ b/2024_2025_proj_auto_avaliacao.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Desktop/Universidade/Computer-Networks-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFB9C07-98F5-5F4B-A0F1-8559CD1F9D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3A29F6-C552-D840-A76B-B412CE06E424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Autoavaliação" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
   <si>
     <t>Ficha de autoavaliação</t>
   </si>
@@ -379,9 +379,6 @@
   </si>
   <si>
     <t>RC11L04</t>
-  </si>
-  <si>
-    <t>TO DO</t>
   </si>
 </sst>
 </file>
@@ -924,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="194" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:E25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="194" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -986,7 +983,7 @@
       </c>
       <c r="B7" s="15">
         <f>B8+F8</f>
-        <v>19</v>
+        <v>18.5</v>
       </c>
       <c r="C7" s="7">
         <f>C8+G8</f>
@@ -1004,7 +1001,7 @@
       </c>
       <c r="B8" s="7">
         <f>SUM(B9:B23)</f>
-        <v>10</v>
+        <v>9.75</v>
       </c>
       <c r="C8" s="7">
         <f>SUM(C9:C23)</f>
@@ -1015,7 +1012,7 @@
       </c>
       <c r="F8" s="7">
         <f>SUM(F9:F23)</f>
-        <v>9</v>
+        <v>8.75</v>
       </c>
       <c r="G8" s="7">
         <f>SUM(G9:G23)</f>
@@ -1212,7 +1209,7 @@
         <v>58</v>
       </c>
       <c r="B21" s="11">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="C21" s="4">
         <v>2</v>
@@ -1221,7 +1218,7 @@
         <v>65</v>
       </c>
       <c r="F21" s="11">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="G21" s="4">
         <v>1.5</v>
@@ -1233,9 +1230,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="43.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
-        <v>76</v>
-      </c>
+      <c r="A25" s="19"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>

</xml_diff>